<commit_message>
fix excel delay 1
</commit_message>
<xml_diff>
--- a/excel_files/data.xlsx
+++ b/excel_files/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,15 +470,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -4398,6 +4390,80 @@
       <c r="G108" t="inlineStr">
         <is>
           <t>https://ar.wikipedia.org/wiki/%D8%A7%D9%84%D8%B3%D8%B9%D9%88%D8%AF%D9%8A%D8%A9</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>test create</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>omar</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>egypt</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D8%B5%D9%86%D8%B9_%D8%A7%D9%84%D9%84%D9%87_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%B5%D8%B1</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%B5%D8%B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>test create</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>omar</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>egypt</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D8%B5%D9%86%D8%B9_%D8%A7%D9%84%D9%84%D9%87_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%B5%D8%B1</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%B5%D8%B1</t>
         </is>
       </c>
     </row>

</xml_diff>